<commit_message>
changed the column headings for programming purposes
</commit_message>
<xml_diff>
--- a/Data/Datasets/AU Final.xlsx
+++ b/Data/Datasets/AU Final.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER-PC\Deakin University\Data 2 Intelligence Consulting - PG - Australia's recession prediction\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\companyandngo\Data\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{741F1D07-70CA-4116-8AF8-FF08AF40E230}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{7F57389A-9876-4F81-9318-2C883E588D6F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{728B7BFE-33B2-4DB0-BAA8-F2EB8366DF80}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3480" yWindow="2856" windowWidth="11520" windowHeight="9588" xr2:uid="{3D95DEDE-05E2-4BF9-B4D0-C3495CB5EA1E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3D95DEDE-05E2-4BF9-B4D0-C3495CB5EA1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -34,25 +34,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
-    <t>Dates</t>
-  </si>
-  <si>
     <t>Recession</t>
   </si>
   <si>
     <t>AORD_monthly_adj_closed</t>
-  </si>
-  <si>
-    <t>Bond Yields: 10-year</t>
-  </si>
-  <si>
-    <t>Unemployment rate</t>
-  </si>
-  <si>
-    <t>3-month Yields</t>
-  </si>
-  <si>
-    <t>The 10 Year-3 Month Treasury Yield Spread</t>
   </si>
   <si>
     <t>monthly date</t>
@@ -74,6 +59,21 @@
   </si>
   <si>
     <t>3-Month or 90-day Rates and Yields: Interbank Rates for Australia(Bank Bills for Australia), Percent, Monthly, Not Seasonally Adjusted</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>10Y_Bond_Yields</t>
+  </si>
+  <si>
+    <t>3M_Bond_Yields</t>
+  </si>
+  <si>
+    <t>3M_10Y_Treasury_Spread</t>
+  </si>
+  <si>
+    <t>Unemployment_Rate</t>
   </si>
 </sst>
 </file>
@@ -2831,7 +2831,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>The 10 Year-3 Month Treasury Yield Spread</c:v>
+                  <c:v>3M_10Y_Treasury_Spread</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6178,15 +6178,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1828800</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>11430</xdr:rowOff>
+      <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1760220</xdr:colOff>
+      <xdr:colOff>297180</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:rowOff>22860</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6514,7 +6514,7 @@
   <dimension ref="A1:G775"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6530,25 +6530,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>6</v>
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
       </c>
       <c r="G1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -18232,7 +18232,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18243,58 +18243,58 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>6</v>
+      <c r="A6" t="s">
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -18303,6 +18303,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006EFE272B2DF4B44EA6E332E22EB86DD4" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7b4c9bdf068468c71ea5f12673ba52d5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="afc71e28-3a3c-4a48-b14a-5eb4c2135c62" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c115a55776667cc25f628bf2cf7532f5" ns2:_="">
     <xsd:import namespace="afc71e28-3a3c-4a48-b14a-5eb4c2135c62"/>
@@ -18486,22 +18501,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96CC5D89-09D7-472C-A41B-629069E11CF6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="afc71e28-3a3c-4a48-b14a-5eb4c2135c62"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A254B8A6-5E67-4F5E-8F8A-E863BD56E96C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E0326E7-EBBB-42A7-8731-5CC70CA93E72}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18517,28 +18541,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A254B8A6-5E67-4F5E-8F8A-E863BD56E96C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96CC5D89-09D7-472C-A41B-629069E11CF6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="afc71e28-3a3c-4a48-b14a-5eb4c2135c62"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>